<commit_message>
Se agrego modulo configuracion y generacion de ´pdf_guia
</commit_message>
<xml_diff>
--- a/utils/docs/FORMATO_PARA_CARGAR_CATEGORIAS.xlsx
+++ b/utils/docs/FORMATO_PARA_CARGAR_CATEGORIAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aistermcon\utils\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241C37F0-C908-44B7-96FE-E90BEB508F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE5D0DF-2990-4603-9C63-BC6E6BD09224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="225" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>